<commit_message>
study 2 analysis update
</commit_message>
<xml_diff>
--- a/study2/presentation_for_paper/study2a_linear_regression_assumption_test.xlsx
+++ b/study2/presentation_for_paper/study2a_linear_regression_assumption_test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2d319992da703ee6/Desktop/Master Thesis/master_thesis/study2/presentation_for_paper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="72" documentId="8_{04B51B2C-F939-4250-9555-F45FDE986B7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4555D463-41AC-4EEB-B47B-E72FB138EB55}"/>
+  <xr:revisionPtr revIDLastSave="81" documentId="8_{04B51B2C-F939-4250-9555-F45FDE986B7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{502744B8-A664-4445-9FEB-932CA9AD9CF1}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{55AC8A10-C792-40F2-8B60-D94B7E634E3F}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>Id</t>
     <phoneticPr fontId="2"/>
@@ -63,10 +63,6 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>Shapiro-Wilk test</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>Variance Inflation Factors (VIF)</t>
     <phoneticPr fontId="2"/>
   </si>
@@ -104,6 +100,14 @@
   </si>
   <si>
     <t>Linearlity</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Visual Assessment though QQ-plot</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Majority of residuals within the 95% CI</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -215,22 +219,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>222250</xdr:colOff>
+      <xdr:colOff>228600</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>107950</xdr:rowOff>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>133350</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>88900</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
+        <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2538488E-EB6D-4201-A087-4883A336B532}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EF675655-18B2-4090-1F70-D0AFDC5E56BD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -253,8 +257,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="222250" y="107950"/>
-          <a:ext cx="6515100" cy="1111250"/>
+          <a:off x="228600" y="133350"/>
+          <a:ext cx="7124700" cy="1111250"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -600,13 +604,15 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D6" sqref="A1:D6"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="3.6640625" style="1" customWidth="1"/>
-    <col min="2" max="4" width="27.25" style="1" customWidth="1"/>
+    <col min="2" max="2" width="27.25" style="1" customWidth="1"/>
+    <col min="3" max="3" width="29.1640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="33.33203125" style="1" customWidth="1"/>
     <col min="5" max="16384" width="8.6640625" style="1"/>
   </cols>
   <sheetData>
@@ -615,13 +621,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>11</v>
-      </c>
       <c r="D1" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -629,13 +635,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -643,13 +649,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -663,7 +669,7 @@
         <v>5</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -674,10 +680,10 @@
         <v>2</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -688,10 +694,10 @@
         <v>3</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -705,7 +711,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18"/>

</xml_diff>